<commit_message>
bugdet variance fase PDROB
</commit_message>
<xml_diff>
--- a/Documents/RP/ExternalDocuments/PianoDiQualifica/resoconto.xlsx
+++ b/Documents/RP/ExternalDocuments/PianoDiQualifica/resoconto.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Federico\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Federico\Documents\GitHub\Leaf\Documents\RP\ExternalDocuments\PianoDiQualifica\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>Documenti</t>
   </si>
@@ -117,14 +117,28 @@
   </si>
   <si>
     <t>Costo</t>
+  </si>
+  <si>
+    <t>DP</t>
+  </si>
+  <si>
+    <t>Programmatore</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -269,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -280,9 +294,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -290,9 +301,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -353,6 +361,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -633,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:L23"/>
+  <dimension ref="C3:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,530 +679,569 @@
   <sheetData>
     <row r="3" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="29" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="24">
         <v>30</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="7">
-        <v>10</v>
-      </c>
-      <c r="G5" s="7">
-        <v>-1</v>
-      </c>
-      <c r="H5" s="7">
-        <f t="shared" ref="H5:H11" si="0">(G5/F5)*100</f>
-        <v>-10</v>
-      </c>
-      <c r="I5" s="7" t="str">
+      <c r="F5" s="24">
+        <v>20</v>
+      </c>
+      <c r="G5" s="24">
+        <v>-8</v>
+      </c>
+      <c r="H5" s="24">
+        <f t="shared" ref="H5:H12" si="0">(G5/F5)*100</f>
+        <v>-40</v>
+      </c>
+      <c r="I5" s="24" t="str">
         <f>IF(H5&lt;=0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="J5" s="7" t="str">
+      <c r="J5" s="24" t="str">
         <f>IF(AND(H5&gt;0,H5&lt;=10),"X","")</f>
         <v/>
       </c>
-      <c r="K5" s="8" t="str">
+      <c r="K5" s="25" t="str">
         <f>IF(H5&gt;10,"X","")</f>
         <v/>
       </c>
     </row>
     <row r="6" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="24">
         <v>20</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="7">
-        <v>17</v>
-      </c>
-      <c r="G6" s="7">
-        <v>-1</v>
-      </c>
-      <c r="H6" s="7">
+      <c r="F6" s="24">
+        <v>2</v>
+      </c>
+      <c r="G6" s="24">
+        <v>0</v>
+      </c>
+      <c r="H6" s="24">
         <f t="shared" si="0"/>
-        <v>-5.8823529411764701</v>
-      </c>
-      <c r="I6" s="7" t="str">
+        <v>0</v>
+      </c>
+      <c r="I6" s="24" t="str">
         <f>IF(H6&lt;=0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="J6" s="7" t="str">
+      <c r="J6" s="24" t="str">
         <f>IF(AND(H6&gt;0,H6&lt;=10),"X","")</f>
         <v/>
       </c>
-      <c r="K6" s="8" t="str">
+      <c r="K6" s="25" t="str">
         <f>IF(H6&gt;10,"X","")</f>
         <v/>
       </c>
     </row>
     <row r="7" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="24">
         <v>25</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="7">
-        <v>2</v>
-      </c>
-      <c r="G7" s="7">
+      <c r="F7" s="24">
+        <v>3</v>
+      </c>
+      <c r="G7" s="24">
         <v>0</v>
       </c>
-      <c r="H7" s="26">
+      <c r="H7" s="30">
         <f>(((G8/F8)*D8+(G7/F7)*D7)/45)*100</f>
         <v>-22.222222222222221</v>
       </c>
-      <c r="I7" s="26" t="str">
+      <c r="I7" s="30" t="str">
         <f>IF(H7&lt;=0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="J7" s="26" t="str">
+      <c r="J7" s="30" t="str">
         <f>IF(AND(H7&gt;0,H7&lt;=10),"X","")</f>
         <v/>
       </c>
-      <c r="K7" s="27" t="str">
+      <c r="K7" s="31" t="str">
         <f>IF(H7&gt;10,"X","")</f>
         <v/>
       </c>
     </row>
     <row r="8" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="24">
         <v>20</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="24">
         <v>2</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="24">
         <v>-1</v>
       </c>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="27"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="31"/>
     </row>
     <row r="9" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="24">
         <v>25</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="7">
-        <v>72</v>
-      </c>
-      <c r="G9" s="7">
-        <v>-10</v>
-      </c>
-      <c r="H9" s="7">
+      <c r="F9" s="24">
+        <v>24</v>
+      </c>
+      <c r="G9" s="24">
+        <v>-15</v>
+      </c>
+      <c r="H9" s="24">
         <f t="shared" si="0"/>
-        <v>-13.888888888888889</v>
-      </c>
-      <c r="I9" s="7" t="str">
+        <v>-62.5</v>
+      </c>
+      <c r="I9" s="24" t="str">
         <f>IF(H9&lt;=0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="J9" s="7" t="str">
+      <c r="J9" s="24" t="str">
         <f>IF(AND(H9&gt;0,H9&lt;=10),"X","")</f>
         <v/>
       </c>
-      <c r="K9" s="8" t="str">
+      <c r="K9" s="25" t="str">
         <f>IF(H9&gt;10,"X","")</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="24">
         <v>25</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="23">
         <v>1</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="24">
         <v>0</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I10" s="7" t="str">
+      <c r="I10" s="24" t="str">
         <f>IF(H10&lt;=0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="J10" s="7" t="str">
+      <c r="J10" s="24" t="str">
         <f>IF(AND(H10&gt;0,H10&lt;=10),"X","")</f>
         <v/>
       </c>
-      <c r="K10" s="8" t="str">
+      <c r="K10" s="25" t="str">
         <f>IF(H10&gt;10,"X","")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="10">
+    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="24">
         <v>22</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="10">
-        <v>45</v>
-      </c>
-      <c r="G11" s="10">
-        <v>7</v>
-      </c>
-      <c r="H11" s="10">
+      <c r="F11" s="24">
+        <v>62</v>
+      </c>
+      <c r="G11" s="24">
+        <v>36</v>
+      </c>
+      <c r="H11" s="24">
         <f t="shared" si="0"/>
-        <v>15.555555555555555</v>
-      </c>
-      <c r="I11" s="10" t="str">
+        <v>58.064516129032263</v>
+      </c>
+      <c r="I11" s="24" t="str">
         <f>IF(H11&lt;=0,"X","")</f>
         <v/>
       </c>
-      <c r="J11" s="10" t="str">
+      <c r="J11" s="24" t="str">
         <f>IF(AND(H11&gt;0,H11&lt;=10),"X","")</f>
         <v/>
       </c>
-      <c r="K11" s="11" t="str">
+      <c r="K11" s="25" t="str">
         <f>IF(H11&gt;10,"X","")</f>
         <v>X</v>
       </c>
     </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1" t="s">
+    <row r="12" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="8">
+        <v>15</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="8">
+        <v>15</v>
+      </c>
+      <c r="G12" s="8">
+        <v>-2</v>
+      </c>
+      <c r="H12" s="8">
+        <f t="shared" si="0"/>
+        <v>-13.333333333333334</v>
+      </c>
+      <c r="I12" s="8" t="str">
+        <f>IF(H12&lt;=0,"X","")</f>
+        <v>X</v>
+      </c>
+      <c r="J12" s="8" t="str">
+        <f>IF(AND(H12&gt;0,H12&lt;=10),"X","")</f>
+        <v/>
+      </c>
+      <c r="K12" s="9" t="str">
+        <f>IF(H12&gt;10,"X","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="7">
-        <f>SUM(D5*G5,D6*G6,D7*G7,D8*G8,D9*G9,D10*G10,D11*G11)/SUM(D5*F5,D6*F6,D7*F7,D8*F8,D9*F9,D10*F10,D11*F11)*100</f>
-        <v>-4.6826516220028207</v>
-      </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7" t="str">
-        <f>IF(H12&gt;10,"X","")</f>
-        <v/>
-      </c>
-      <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K13" s="28"/>
-      <c r="L13" s="7"/>
+      <c r="H13" s="6">
+        <f>(SUM(D5*G5,D6*G6,D7*G7,D8*G8,D9*G9,D10*G10,D11*G11,D12*G12)/SUM(D5*F5,D6*F6,D7*F7,D8*F8,D9*F9,D10*F10,D11*F11,D12*F12))*100</f>
+        <v>4.2775345234085549</v>
+      </c>
+      <c r="I13" s="8" t="str">
+        <f>IF(H13&lt;=0,"X","")</f>
+        <v/>
+      </c>
+      <c r="J13" s="8" t="str">
+        <f>IF(AND(H13&gt;0,H13&lt;=10),"X","")</f>
+        <v>X</v>
+      </c>
+      <c r="K13" s="9" t="str">
+        <f>IF(H13&gt;10,"X","")</f>
+        <v/>
+      </c>
+      <c r="L13" s="1"/>
     </row>
     <row r="14" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="12" t="s">
+      <c r="K14" s="26"/>
+      <c r="L14" s="6"/>
+    </row>
+    <row r="15" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13" t="s">
+      <c r="D15" s="11"/>
+      <c r="E15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="13">
-        <v>18</v>
-      </c>
-      <c r="G14" s="13">
-        <v>-4</v>
-      </c>
-      <c r="H14" s="13">
-        <f>(G14/F14)*100</f>
-        <v>-22.222222222222221</v>
-      </c>
-      <c r="I14" s="13" t="str">
-        <f>IF(H14&lt;=0,"X","")</f>
+      <c r="F15" s="11">
+        <v>20</v>
+      </c>
+      <c r="G15" s="11">
+        <v>-2</v>
+      </c>
+      <c r="H15" s="11">
+        <f>(G15/F15)*100</f>
+        <v>-10</v>
+      </c>
+      <c r="I15" s="11" t="str">
+        <f>IF(H15&lt;=0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="J14" s="13" t="str">
-        <f>IF(AND(H14&gt;0,H14&lt;=10),"X","")</f>
-        <v/>
-      </c>
-      <c r="K14" s="14" t="str">
-        <f>IF(H14&gt;10,"X","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="3:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="C16" s="2" t="s">
+      <c r="J15" s="11" t="str">
+        <f>IF(AND(H15&gt;0,H15&lt;=10),"X","")</f>
+        <v/>
+      </c>
+      <c r="K15" s="12" t="str">
+        <f>IF(H15&gt;10,"X","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="3:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E17" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F17" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G17" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="18" t="s">
+      <c r="H17" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="18" t="s">
+      <c r="I17" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="17" t="s">
+      <c r="J17" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="K16" s="19" t="s">
+      <c r="K17" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C17" s="5" t="s">
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C18" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D18" s="5">
         <v>5</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E18" s="18">
         <v>42441</v>
       </c>
-      <c r="F17" s="20">
+      <c r="F18" s="18">
         <v>42441</v>
       </c>
-      <c r="G17" s="23">
+      <c r="G18" s="21">
         <v>3</v>
       </c>
-      <c r="H17" s="20">
+      <c r="H18" s="18">
         <v>42442</v>
       </c>
-      <c r="I17" s="20">
+      <c r="I18" s="18">
         <v>42442</v>
       </c>
-      <c r="J17" s="23">
-        <f>(F17-E17)/D17*100</f>
+      <c r="J18" s="21">
+        <f>(F18-E18)/D18*100</f>
         <v>0</v>
       </c>
-      <c r="K17" s="21">
-        <f>(I17-H17)/G17*100</f>
+      <c r="K18" s="19">
+        <f>(I18-H18)/G18*100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C18" s="5" t="s">
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C19" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D19" s="5">
         <v>3</v>
       </c>
-      <c r="E18" s="20">
+      <c r="E19" s="18">
         <v>42424</v>
       </c>
-      <c r="F18" s="20">
+      <c r="F19" s="18">
         <v>42425</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G19" s="5">
         <v>2</v>
       </c>
-      <c r="H18" s="20">
+      <c r="H19" s="18">
         <v>42426</v>
       </c>
-      <c r="I18" s="20">
+      <c r="I19" s="18">
         <v>42426</v>
       </c>
-      <c r="J18" s="23">
-        <f t="shared" ref="J18:J22" si="1">(F18-E18)/D18*100</f>
+      <c r="J19" s="21">
+        <f t="shared" ref="J19:J23" si="1">(F19-E19)/D19*100</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="K18" s="21">
-        <f t="shared" ref="K18:K22" si="2">(I18-H18)/G18*100</f>
+      <c r="K19" s="19">
+        <f t="shared" ref="K19:K23" si="2">(I19-H19)/G19*100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C19" s="5" t="s">
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D20" s="5">
         <v>4</v>
       </c>
-      <c r="E19" s="20">
+      <c r="E20" s="18">
         <v>42442</v>
       </c>
-      <c r="F19" s="20">
+      <c r="F20" s="18">
         <v>42442</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G20" s="5">
         <v>2</v>
       </c>
-      <c r="H19" s="20">
+      <c r="H20" s="18">
         <v>42442</v>
       </c>
-      <c r="I19" s="16">
+      <c r="I20" s="14">
         <v>42442</v>
       </c>
-      <c r="J19" s="23">
+      <c r="J20" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K19" s="21">
-        <f>(I17-H19)/G19*100</f>
+      <c r="K20" s="19">
+        <f>(I18-H20)/G20*100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C20" s="5" t="s">
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C21" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D21" s="5">
         <v>4</v>
       </c>
-      <c r="E20" s="20">
+      <c r="E21" s="18">
         <v>42425</v>
       </c>
-      <c r="F20" s="20">
+      <c r="F21" s="18">
         <v>42426</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G21" s="5">
         <v>2</v>
       </c>
-      <c r="H20" s="20">
+      <c r="H21" s="18">
         <v>42427</v>
       </c>
-      <c r="I20" s="20">
+      <c r="I21" s="18">
         <v>42427</v>
       </c>
-      <c r="J20" s="23">
+      <c r="J21" s="21">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="K20" s="21">
+      <c r="K21" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C21" s="5" t="s">
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C22" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D22" s="13">
         <v>18</v>
       </c>
-      <c r="E21" s="20">
+      <c r="E22" s="18">
         <v>42440</v>
       </c>
-      <c r="F21" s="20">
+      <c r="F22" s="18">
         <v>42439</v>
       </c>
-      <c r="G21" s="15">
+      <c r="G22" s="13">
         <v>1</v>
       </c>
-      <c r="H21" s="20">
+      <c r="H22" s="18">
         <v>42442</v>
       </c>
-      <c r="I21" s="20">
+      <c r="I22" s="18">
         <v>42439</v>
       </c>
-      <c r="J21" s="23">
+      <c r="J22" s="21">
         <f t="shared" si="1"/>
         <v>-5.5555555555555554</v>
       </c>
-      <c r="K21" s="21">
+      <c r="K22" s="19">
         <f t="shared" si="2"/>
         <v>-300</v>
       </c>
     </row>
-    <row r="22" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="9" t="s">
+    <row r="23" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D23" s="8">
         <v>18</v>
       </c>
-      <c r="E22" s="22">
+      <c r="E23" s="20">
         <v>42440</v>
       </c>
-      <c r="F22" s="22">
+      <c r="F23" s="20">
         <v>42442</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G23" s="8">
         <v>2</v>
       </c>
-      <c r="H22" s="22">
+      <c r="H23" s="20">
         <v>42442</v>
       </c>
-      <c r="I22" s="22">
+      <c r="I23" s="20">
         <v>42443</v>
       </c>
-      <c r="J22" s="23">
+      <c r="J23" s="21">
         <f t="shared" si="1"/>
         <v>11.111111111111111</v>
       </c>
-      <c r="K22" s="21">
+      <c r="K23" s="19">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="I23" t="s">
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
         <v>28</v>
       </c>
-      <c r="K23" s="24">
-        <f>SUM(K17:K22)/6</f>
+      <c r="K24" s="22">
+        <f>SUM(K18:K23)/6</f>
         <v>-41.666666666666664</v>
       </c>
     </row>

</xml_diff>